<commit_message>
main figures draft 1
</commit_message>
<xml_diff>
--- a/experiments/0_ss_finding/time_required.xlsx
+++ b/experiments/0_ss_finding/time_required.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owenpetchey/Desktop/microxanox/diversity_envresp1/experiments/0_ss_finding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B76490-5107-8940-8783-5A472DEEE034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83909006-9787-3847-BAD3-B14B97E2ECF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="2800" windowWidth="43480" windowHeight="21180" xr2:uid="{06D63768-2800-344A-AD80-A7CE429FF153}"/>
+    <workbookView xWindow="8160" yWindow="980" windowWidth="29660" windowHeight="17600" xr2:uid="{06D63768-2800-344A-AD80-A7CE429FF153}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>var_expt length</t>
   </si>
@@ -314,10 +314,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$I$2:$I$13</c:f>
+              <c:f>data!$I$2:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>104166.66666666667</c:v>
                 </c:pt>
@@ -353,16 +353,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>208333333.33333334</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>483333333.33333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$J$2:$J$13</c:f>
+              <c:f>data!$J$2:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>61</c:v>
                 </c:pt>
@@ -398,6 +401,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>21231</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -657,10 +663,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$S$2:$S$12</c:f>
+              <c:f>data!$S$2:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5.017728766960432</c:v>
                 </c:pt>
@@ -693,16 +699,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>8.3187587626244124</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3187587626244124</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.6842467475153118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$T$2:$T$12</c:f>
+              <c:f>data!$T$2:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.7853298350107671</c:v>
                 </c:pt>
@@ -735,6 +747,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4.4800932180589612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3269704503249207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.7403626894942441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2423,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1196A045-20BB-3147-9839-C23564CDEFB5}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3062,11 +3080,11 @@
         <v>25951.898740120923</v>
       </c>
       <c r="S11">
-        <f t="shared" ref="S11:S13" si="13">LOG10(I11)</f>
+        <f t="shared" ref="S11:S14" si="13">LOG10(I11)</f>
         <v>8.3187587626244124</v>
       </c>
       <c r="T11">
-        <f t="shared" ref="T11:T13" si="14">LOG10(J11)</f>
+        <f t="shared" ref="T11:T14" si="14">LOG10(J11)</f>
         <v>4.4640422054388109</v>
       </c>
       <c r="U11" s="1"/>
@@ -3092,7 +3110,7 @@
         <v>100000000</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G13" si="15" xml:space="preserve"> IF(C12&lt;12,C12, 12)</f>
+        <f t="shared" ref="G12:G14" si="15" xml:space="preserve"> IF(C12&lt;12,C12, 12)</f>
         <v>12</v>
       </c>
       <c r="H12" s="1">
@@ -3200,15 +3218,68 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="O14" s="1"/>
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1">
+        <f>D14*E14</f>
+        <v>100000000</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="H14" s="1">
+        <f>C14*D14*E14</f>
+        <v>5800000000</v>
+      </c>
+      <c r="I14" s="1">
+        <f>H14/G14</f>
+        <v>483333333.33333331</v>
+      </c>
+      <c r="J14" s="1">
+        <v>55000</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14*regression!B$18+regression!B$17</f>
+        <v>60042.320600512801</v>
+      </c>
+      <c r="L14" s="6">
+        <f>K14/60</f>
+        <v>1000.7053433418801</v>
+      </c>
+      <c r="M14" s="6">
+        <f>L14/60</f>
+        <v>16.678422389031333</v>
+      </c>
+      <c r="N14">
+        <f>M14/24</f>
+        <v>0.69493426620963883</v>
+      </c>
+      <c r="O14" s="1">
+        <f>I14*regression!B$18+regression!B$17</f>
+        <v>60042.320600512801</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="13"/>
+        <v>8.6842467475153118</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="14"/>
+        <v>4.7403626894942441</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D15" s="1"/>

</xml_diff>